<commit_message>
redesign architecture for sqlite, imporve convert and update scripts, bugfixes
</commit_message>
<xml_diff>
--- a/converter/tournaments_base.xlsx
+++ b/converter/tournaments_base.xlsx
@@ -9590,8 +9590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1249" workbookViewId="0">
-      <selection activeCell="A1268" sqref="A1268"/>
+    <sheetView tabSelected="1" topLeftCell="A1155" workbookViewId="0">
+      <selection activeCell="E1176" sqref="E1176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78911,9 +78911,7 @@
       <c r="R1309" s="5">
         <v>8</v>
       </c>
-      <c r="S1309" s="6">
-        <v>317794</v>
-      </c>
+      <c r="S1309" s="6"/>
       <c r="T1309" s="5" t="s">
         <v>35</v>
       </c>

</xml_diff>